<commit_message>
API for feedback success
</commit_message>
<xml_diff>
--- a/backend/excel/feedback-db.xlsx
+++ b/backend/excel/feedback-db.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>No</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>good service</t>
   </si>
 </sst>
 </file>
@@ -377,7 +380,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -417,6 +420,20 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Success creating API for employee, patient, modified feedback
</commit_message>
<xml_diff>
--- a/backend/excel/feedback-db.xlsx
+++ b/backend/excel/feedback-db.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>No</t>
   </si>
@@ -38,6 +38,15 @@
   </si>
   <si>
     <t>good service</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>excellent service</t>
+  </si>
+  <si>
+    <t>nice service</t>
   </si>
 </sst>
 </file>
@@ -380,7 +389,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -434,6 +443,34 @@
         <v>6</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
implemented feedback form modal, modified contents of feedback script and the context
</commit_message>
<xml_diff>
--- a/backend/excel/feedback-db.xlsx
+++ b/backend/excel/feedback-db.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>No</t>
   </si>
@@ -25,28 +25,25 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Verification</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>good</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>good service</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>excellent service</t>
-  </si>
-  <si>
-    <t>nice service</t>
+    <t>very satisfied</t>
+  </si>
+  <si>
+    <t>very nive experience</t>
+  </si>
+  <si>
+    <t>neutral</t>
+  </si>
+  <si>
+    <t>love it!</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>unsatisfied</t>
+  </si>
+  <si>
+    <t>atif</t>
   </si>
 </sst>
 </file>
@@ -54,13 +51,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -71,7 +74,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -83,9 +93,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" borderId="1" applyBorder="1" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" borderId="1" applyBorder="1" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -389,86 +409,65 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="1" width="13.576428571428572" customWidth="1" style="2"/>
-    <col min="2" max="2" bestFit="1" width="13.576428571428572" customWidth="1" style="2"/>
-    <col min="3" max="3" bestFit="1" width="13.576428571428572" customWidth="1" style="2"/>
-    <col min="4" max="4" bestFit="1" width="13.576428571428572" customWidth="1" style="2"/>
+    <col min="1" max="1" bestFit="1" width="13.576428571428572" customWidth="1" style="4"/>
+    <col min="2" max="2" bestFit="1" width="13.576428571428572" customWidth="1" style="5"/>
+    <col min="3" max="3" bestFit="1" width="13.576428571428572" customWidth="1" style="6"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" ht="18.75" customHeight="1">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>7</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>6</v>
+      <c r="D4" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>